<commit_message>
Update Barchart, Biểu mẫu, Yêu cầu. Tạo Use Case Format
Use Case Format mẫu nằm trong thư mục Phân Tích/UseCases
</commit_message>
<xml_diff>
--- a/Phân tích/Barchart.xlsx
+++ b/Phân tích/Barchart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CNPM\Phân tích\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Homework\CN Phan Mem\Homework\CNPM\Phân tích\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A96111-06C1-45BB-B2A5-37029FF95D37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76B6797-B9B3-4A3E-931F-22A4E04CE388}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="66">
   <si>
     <t>Quản lí nhân viên</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>- Tài khoản</t>
+  </si>
+  <si>
+    <t>- Xem thông tin khách hàng</t>
   </si>
 </sst>
 </file>
@@ -692,23 +695,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T50"/>
+  <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="4" width="9.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="16" width="9.140625" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="29.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="1"/>
+    <col min="3" max="4" width="9.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="1"/>
+    <col min="6" max="16" width="9.109375" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>30</v>
       </c>
@@ -717,7 +720,7 @@
       <c r="D1" s="20"/>
       <c r="E1" s="20"/>
     </row>
-    <row r="2" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D2" s="5"/>
       <c r="E2" s="21" t="s">
         <v>46</v>
@@ -741,7 +744,7 @@
       <c r="R2"/>
       <c r="S2"/>
     </row>
-    <row r="3" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D3" s="7" t="s">
         <v>41</v>
       </c>
@@ -786,7 +789,7 @@
       <c r="S3" s="6"/>
       <c r="T3" s="6"/>
     </row>
-    <row r="4" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>31</v>
       </c>
@@ -795,7 +798,7 @@
       </c>
       <c r="O4"/>
     </row>
-    <row r="5" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -822,7 +825,7 @@
       <c r="S5" s="8"/>
       <c r="T5" s="8"/>
     </row>
-    <row r="6" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -851,7 +854,7 @@
       <c r="S6" s="8"/>
       <c r="T6" s="8"/>
     </row>
-    <row r="7" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -880,7 +883,7 @@
       <c r="S7" s="8"/>
       <c r="T7" s="8"/>
     </row>
-    <row r="8" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -909,7 +912,7 @@
       <c r="S8" s="8"/>
       <c r="T8" s="8"/>
     </row>
-    <row r="9" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19" t="s">
         <v>60</v>
       </c>
@@ -936,7 +939,7 @@
       <c r="S9" s="8"/>
       <c r="T9" s="8"/>
     </row>
-    <row r="10" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>61</v>
       </c>
@@ -955,7 +958,7 @@
       <c r="S10" s="8"/>
       <c r="T10" s="8"/>
     </row>
-    <row r="11" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>62</v>
       </c>
@@ -974,7 +977,7 @@
       <c r="S11" s="8"/>
       <c r="T11" s="8"/>
     </row>
-    <row r="12" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>59</v>
       </c>
@@ -993,7 +996,7 @@
       <c r="S12" s="8"/>
       <c r="T12" s="8"/>
     </row>
-    <row r="13" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -1019,7 +1022,7 @@
       <c r="S13" s="8"/>
       <c r="T13" s="8"/>
     </row>
-    <row r="14" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -1047,7 +1050,7 @@
       <c r="S14" s="8"/>
       <c r="T14" s="8"/>
     </row>
-    <row r="15" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>57</v>
       </c>
@@ -1075,7 +1078,7 @@
       <c r="S15" s="8"/>
       <c r="T15" s="8"/>
     </row>
-    <row r="16" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -1103,7 +1106,7 @@
       <c r="S16" s="8"/>
       <c r="T16" s="8"/>
     </row>
-    <row r="17" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -1131,7 +1134,7 @@
       <c r="S17" s="8"/>
       <c r="T17" s="8"/>
     </row>
-    <row r="18" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
@@ -1159,7 +1162,7 @@
       <c r="S18" s="8"/>
       <c r="T18" s="8"/>
     </row>
-    <row r="19" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>64</v>
       </c>
@@ -1188,7 +1191,7 @@
       <c r="S19" s="8"/>
       <c r="T19" s="8"/>
     </row>
-    <row r="20" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
@@ -1214,7 +1217,7 @@
       <c r="S20" s="8"/>
       <c r="T20" s="8"/>
     </row>
-    <row r="21" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
@@ -1242,7 +1245,7 @@
       <c r="S21" s="8"/>
       <c r="T21" s="8"/>
     </row>
-    <row r="22" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
@@ -1270,7 +1273,7 @@
       <c r="S22" s="8"/>
       <c r="T22" s="8"/>
     </row>
-    <row r="23" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>10</v>
       </c>
@@ -1298,7 +1301,7 @@
       <c r="S23" s="8"/>
       <c r="T23" s="8"/>
     </row>
-    <row r="24" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
@@ -1325,7 +1328,7 @@
       <c r="S24" s="8"/>
       <c r="T24" s="8"/>
     </row>
-    <row r="25" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
@@ -1354,7 +1357,7 @@
       <c r="S25" s="8"/>
       <c r="T25" s="8"/>
     </row>
-    <row r="26" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
@@ -1383,7 +1386,7 @@
       <c r="S26" s="8"/>
       <c r="T26" s="8"/>
     </row>
-    <row r="27" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
@@ -1412,7 +1415,7 @@
       <c r="S27" s="8"/>
       <c r="T27" s="8"/>
     </row>
-    <row r="28" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>5</v>
       </c>
@@ -1441,7 +1444,7 @@
       <c r="S28" s="8"/>
       <c r="T28" s="8"/>
     </row>
-    <row r="29" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>23</v>
       </c>
@@ -1470,7 +1473,7 @@
       <c r="S29" s="8"/>
       <c r="T29" s="8"/>
     </row>
-    <row r="30" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>3</v>
       </c>
@@ -1497,7 +1500,7 @@
       <c r="S30" s="8"/>
       <c r="T30" s="8"/>
     </row>
-    <row r="31" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>13</v>
       </c>
@@ -1526,7 +1529,7 @@
       <c r="S31" s="8"/>
       <c r="T31" s="8"/>
     </row>
-    <row r="32" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>21</v>
       </c>
@@ -1555,7 +1558,7 @@
       <c r="S32" s="8"/>
       <c r="T32" s="8"/>
     </row>
-    <row r="33" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>14</v>
       </c>
@@ -1584,7 +1587,7 @@
       <c r="S33" s="8"/>
       <c r="T33" s="8"/>
     </row>
-    <row r="34" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>15</v>
       </c>
@@ -1611,7 +1614,7 @@
       <c r="S34" s="8"/>
       <c r="T34" s="8"/>
     </row>
-    <row r="35" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>16</v>
       </c>
@@ -1640,7 +1643,7 @@
       <c r="S35" s="8"/>
       <c r="T35" s="8"/>
     </row>
-    <row r="36" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>18</v>
       </c>
@@ -1669,7 +1672,7 @@
       <c r="S36" s="8"/>
       <c r="T36" s="8"/>
     </row>
-    <row r="37" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>20</v>
       </c>
@@ -1698,7 +1701,7 @@
       <c r="S37" s="8"/>
       <c r="T37" s="8"/>
     </row>
-    <row r="38" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>22</v>
       </c>
@@ -1725,7 +1728,7 @@
       <c r="S38" s="8"/>
       <c r="T38" s="8"/>
     </row>
-    <row r="39" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>24</v>
       </c>
@@ -1754,7 +1757,7 @@
       <c r="S39" s="8"/>
       <c r="T39" s="8"/>
     </row>
-    <row r="40" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>17</v>
       </c>
@@ -1782,7 +1785,7 @@
       <c r="S40" s="8"/>
       <c r="T40" s="8"/>
     </row>
-    <row r="41" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>25</v>
       </c>
@@ -1811,7 +1814,7 @@
       <c r="S41" s="8"/>
       <c r="T41" s="8"/>
     </row>
-    <row r="42" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>26</v>
       </c>
@@ -1840,7 +1843,7 @@
       <c r="S42" s="8"/>
       <c r="T42" s="8"/>
     </row>
-    <row r="43" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>27</v>
       </c>
@@ -1867,7 +1870,7 @@
       <c r="S43" s="8"/>
       <c r="T43" s="8"/>
     </row>
-    <row r="44" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>28</v>
       </c>
@@ -1897,9 +1900,9 @@
       <c r="S44" s="8"/>
       <c r="T44" s="8"/>
     </row>
-    <row r="45" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>33</v>
@@ -1914,10 +1917,10 @@
       <c r="H45" s="8"/>
       <c r="I45" s="8"/>
       <c r="J45" s="8"/>
-      <c r="K45" s="12"/>
-      <c r="L45" s="12"/>
+      <c r="K45" s="17"/>
+      <c r="L45" s="17"/>
       <c r="M45" s="8" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="N45" s="8"/>
       <c r="O45" s="8"/>
@@ -1928,25 +1931,27 @@
       <c r="T45" s="8"/>
     </row>
     <row r="46" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
-        <v>49</v>
+      <c r="A46" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
       <c r="H46" s="8"/>
       <c r="I46" s="8"/>
       <c r="J46" s="8"/>
-      <c r="K46" s="8"/>
-      <c r="L46" s="8"/>
-      <c r="M46" s="8"/>
+      <c r="K46" s="12"/>
+      <c r="L46" s="12"/>
+      <c r="M46" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="N46" s="8"/>
       <c r="O46" s="8"/>
       <c r="P46" s="8"/>
@@ -1955,20 +1960,18 @@
       <c r="S46" s="8"/>
       <c r="T46" s="8"/>
     </row>
-    <row r="47" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>33</v>
+    <row r="47" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D47" s="10"/>
-      <c r="E47" s="8" t="s">
-        <v>52</v>
-      </c>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
@@ -1985,9 +1988,9 @@
       <c r="S47" s="8"/>
       <c r="T47" s="8"/>
     </row>
-    <row r="48" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>33</v>
@@ -1995,11 +1998,11 @@
       <c r="C48" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D48" s="8"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="8" t="s">
-        <v>53</v>
-      </c>
+      <c r="D48" s="10"/>
+      <c r="E48" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F48" s="8"/>
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
       <c r="I48" s="8"/>
@@ -2015,33 +2018,63 @@
       <c r="S48" s="8"/>
       <c r="T48" s="8"/>
     </row>
-    <row r="49" spans="1:16" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D49" s="8"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8"/>
+      <c r="L49" s="8"/>
+      <c r="M49" s="8"/>
+      <c r="N49" s="8"/>
+      <c r="O49" s="8"/>
+      <c r="P49" s="8"/>
+      <c r="Q49" s="8"/>
+      <c r="R49" s="8"/>
+      <c r="S49" s="8"/>
+      <c r="T49" s="8"/>
+    </row>
+    <row r="50" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B49" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E49" s="14"/>
-      <c r="F49" s="8" t="s">
+      <c r="B50" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E50" s="14"/>
+      <c r="F50" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="P49" s="8"/>
-    </row>
-    <row r="50" spans="1:16" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G50" s="8"/>
-      <c r="H50" s="8"/>
-      <c r="I50" s="8"/>
-      <c r="J50" s="8"/>
-      <c r="K50" s="8"/>
-      <c r="L50" s="8"/>
-      <c r="M50" s="8"/>
-      <c r="N50" s="8"/>
-      <c r="O50" s="8"/>
       <c r="P50" s="8"/>
+    </row>
+    <row r="51" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G51" s="8"/>
+      <c r="H51" s="8"/>
+      <c r="I51" s="8"/>
+      <c r="J51" s="8"/>
+      <c r="K51" s="8"/>
+      <c r="L51" s="8"/>
+      <c r="M51" s="8"/>
+      <c r="N51" s="8"/>
+      <c r="O51" s="8"/>
+      <c r="P51" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
update dfd, biểu mẫu
</commit_message>
<xml_diff>
--- a/Phân tích/Barchart.xlsx
+++ b/Phân tích/Barchart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Homework\CN Phan Mem\Homework\CNPM\Phân tích\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CNPM\Phân tích\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76B6797-B9B3-4A3E-931F-22A4E04CE388}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29CB8E90-D67C-45E4-A552-992AD8B20780}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -180,9 +180,6 @@
     <t>- Đăng nhập</t>
   </si>
   <si>
-    <t>- Thay đổi thông tin tài khoản</t>
-  </si>
-  <si>
     <t>Kim Long</t>
   </si>
   <si>
@@ -223,6 +220,9 @@
   </si>
   <si>
     <t>- Xem thông tin khách hàng</t>
+  </si>
+  <si>
+    <t>- Xem, thay đổi thông tin tài khoản</t>
   </si>
 </sst>
 </file>
@@ -697,21 +697,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="M45" sqref="M45"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" style="1"/>
-    <col min="3" max="4" width="9.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="1"/>
-    <col min="6" max="16" width="9.109375" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="29.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="4" width="9.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="16" width="9.140625" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>30</v>
       </c>
@@ -720,7 +720,7 @@
       <c r="D1" s="20"/>
       <c r="E1" s="20"/>
     </row>
-    <row r="2" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D2" s="5"/>
       <c r="E2" s="21" t="s">
         <v>46</v>
@@ -738,13 +738,13 @@
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
       <c r="P2" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q2"/>
       <c r="R2"/>
       <c r="S2"/>
     </row>
-    <row r="3" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D3" s="7" t="s">
         <v>41</v>
       </c>
@@ -789,7 +789,7 @@
       <c r="S3" s="6"/>
       <c r="T3" s="6"/>
     </row>
-    <row r="4" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>31</v>
       </c>
@@ -798,7 +798,7 @@
       </c>
       <c r="O4"/>
     </row>
-    <row r="5" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -825,7 +825,7 @@
       <c r="S5" s="8"/>
       <c r="T5" s="8"/>
     </row>
-    <row r="6" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -845,7 +845,7 @@
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
       <c r="M6" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>
@@ -854,7 +854,7 @@
       <c r="S6" s="8"/>
       <c r="T6" s="8"/>
     </row>
-    <row r="7" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -874,7 +874,7 @@
       <c r="K7" s="14"/>
       <c r="L7" s="14"/>
       <c r="M7" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
@@ -883,7 +883,7 @@
       <c r="S7" s="8"/>
       <c r="T7" s="8"/>
     </row>
-    <row r="8" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -903,7 +903,7 @@
       <c r="K8" s="14"/>
       <c r="L8" s="14"/>
       <c r="M8" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
@@ -912,9 +912,9 @@
       <c r="S8" s="8"/>
       <c r="T8" s="8"/>
     </row>
-    <row r="9" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>31</v>
@@ -939,9 +939,9 @@
       <c r="S9" s="8"/>
       <c r="T9" s="8"/>
     </row>
-    <row r="10" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>33</v>
@@ -952,15 +952,15 @@
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
       <c r="M10" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q10" s="8"/>
       <c r="S10" s="8"/>
       <c r="T10" s="8"/>
     </row>
-    <row r="11" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>33</v>
@@ -971,15 +971,15 @@
       <c r="K11" s="11"/>
       <c r="L11" s="11"/>
       <c r="M11" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q11" s="8"/>
       <c r="S11" s="8"/>
       <c r="T11" s="8"/>
     </row>
-    <row r="12" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>33</v>
@@ -990,13 +990,13 @@
       <c r="M12" s="18"/>
       <c r="N12" s="18"/>
       <c r="O12" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q12" s="8"/>
       <c r="S12" s="8"/>
       <c r="T12" s="8"/>
     </row>
-    <row r="13" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -1022,7 +1022,7 @@
       <c r="S13" s="8"/>
       <c r="T13" s="8"/>
     </row>
-    <row r="14" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -1034,7 +1034,7 @@
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
@@ -1050,9 +1050,9 @@
       <c r="S14" s="8"/>
       <c r="T14" s="8"/>
     </row>
-    <row r="15" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>33</v>
@@ -1062,7 +1062,7 @@
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
@@ -1078,7 +1078,7 @@
       <c r="S15" s="8"/>
       <c r="T15" s="8"/>
     </row>
-    <row r="16" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -1091,7 +1091,7 @@
       <c r="E16" s="8"/>
       <c r="F16" s="11"/>
       <c r="G16" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
@@ -1106,7 +1106,7 @@
       <c r="S16" s="8"/>
       <c r="T16" s="8"/>
     </row>
-    <row r="17" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -1119,7 +1119,7 @@
       <c r="E17" s="8"/>
       <c r="F17" s="11"/>
       <c r="G17" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
@@ -1134,7 +1134,7 @@
       <c r="S17" s="8"/>
       <c r="T17" s="8"/>
     </row>
-    <row r="18" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
@@ -1148,7 +1148,7 @@
       <c r="F18" s="8"/>
       <c r="G18" s="14"/>
       <c r="H18" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
@@ -1162,9 +1162,9 @@
       <c r="S18" s="8"/>
       <c r="T18" s="8"/>
     </row>
-    <row r="19" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>33</v>
@@ -1180,7 +1180,7 @@
       <c r="I19" s="8"/>
       <c r="J19" s="12"/>
       <c r="K19" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
@@ -1191,7 +1191,7 @@
       <c r="S19" s="8"/>
       <c r="T19" s="8"/>
     </row>
-    <row r="20" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
@@ -1217,7 +1217,7 @@
       <c r="S20" s="8"/>
       <c r="T20" s="8"/>
     </row>
-    <row r="21" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
@@ -1239,13 +1239,13 @@
       <c r="M21" s="8"/>
       <c r="N21" s="13"/>
       <c r="O21" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q21" s="8"/>
       <c r="S21" s="8"/>
       <c r="T21" s="8"/>
     </row>
-    <row r="22" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
@@ -1267,13 +1267,13 @@
       <c r="M22" s="8"/>
       <c r="N22" s="17"/>
       <c r="O22" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q22" s="8"/>
       <c r="S22" s="8"/>
       <c r="T22" s="8"/>
     </row>
-    <row r="23" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>10</v>
       </c>
@@ -1295,13 +1295,13 @@
       <c r="M23" s="8"/>
       <c r="N23" s="17"/>
       <c r="O23" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q23" s="8"/>
       <c r="S23" s="8"/>
       <c r="T23" s="8"/>
     </row>
-    <row r="24" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
@@ -1328,7 +1328,7 @@
       <c r="S24" s="8"/>
       <c r="T24" s="8"/>
     </row>
-    <row r="25" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
@@ -1346,7 +1346,7 @@
       <c r="I25" s="17"/>
       <c r="J25" s="17"/>
       <c r="K25" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
@@ -1357,7 +1357,7 @@
       <c r="S25" s="8"/>
       <c r="T25" s="8"/>
     </row>
-    <row r="26" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
@@ -1375,7 +1375,7 @@
       <c r="I26" s="17"/>
       <c r="J26" s="17"/>
       <c r="K26" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L26" s="8"/>
       <c r="M26" s="8"/>
@@ -1386,7 +1386,7 @@
       <c r="S26" s="8"/>
       <c r="T26" s="8"/>
     </row>
-    <row r="27" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
@@ -1404,7 +1404,7 @@
       <c r="I27" s="17"/>
       <c r="J27" s="17"/>
       <c r="K27" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L27" s="8"/>
       <c r="M27" s="8"/>
@@ -1415,7 +1415,7 @@
       <c r="S27" s="8"/>
       <c r="T27" s="8"/>
     </row>
-    <row r="28" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>5</v>
       </c>
@@ -1433,7 +1433,7 @@
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
       <c r="K28" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L28" s="8"/>
       <c r="M28" s="8"/>
@@ -1444,7 +1444,7 @@
       <c r="S28" s="8"/>
       <c r="T28" s="8"/>
     </row>
-    <row r="29" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>23</v>
       </c>
@@ -1462,7 +1462,7 @@
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
       <c r="K29" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L29" s="8"/>
       <c r="M29" s="8"/>
@@ -1473,7 +1473,7 @@
       <c r="S29" s="8"/>
       <c r="T29" s="8"/>
     </row>
-    <row r="30" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>3</v>
       </c>
@@ -1500,7 +1500,7 @@
       <c r="S30" s="8"/>
       <c r="T30" s="8"/>
     </row>
-    <row r="31" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>13</v>
       </c>
@@ -1520,7 +1520,7 @@
       <c r="K31" s="11"/>
       <c r="L31" s="11"/>
       <c r="M31" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N31" s="8"/>
       <c r="O31" s="8"/>
@@ -1529,7 +1529,7 @@
       <c r="S31" s="8"/>
       <c r="T31" s="8"/>
     </row>
-    <row r="32" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>21</v>
       </c>
@@ -1549,7 +1549,7 @@
       <c r="K32" s="17"/>
       <c r="L32" s="17"/>
       <c r="M32" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N32" s="8"/>
       <c r="O32" s="8"/>
@@ -1558,7 +1558,7 @@
       <c r="S32" s="8"/>
       <c r="T32" s="8"/>
     </row>
-    <row r="33" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>14</v>
       </c>
@@ -1578,7 +1578,7 @@
       <c r="K33" s="17"/>
       <c r="L33" s="17"/>
       <c r="M33" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N33" s="8"/>
       <c r="O33" s="8"/>
@@ -1587,7 +1587,7 @@
       <c r="S33" s="8"/>
       <c r="T33" s="8"/>
     </row>
-    <row r="34" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>15</v>
       </c>
@@ -1614,7 +1614,7 @@
       <c r="S34" s="8"/>
       <c r="T34" s="8"/>
     </row>
-    <row r="35" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>16</v>
       </c>
@@ -1631,7 +1631,7 @@
       <c r="H35" s="13"/>
       <c r="I35" s="13"/>
       <c r="J35" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K35" s="8"/>
       <c r="L35" s="8"/>
@@ -1643,7 +1643,7 @@
       <c r="S35" s="8"/>
       <c r="T35" s="8"/>
     </row>
-    <row r="36" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>18</v>
       </c>
@@ -1661,7 +1661,7 @@
       <c r="I36" s="8"/>
       <c r="J36" s="12"/>
       <c r="K36" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L36" s="8"/>
       <c r="M36" s="8"/>
@@ -1672,7 +1672,7 @@
       <c r="S36" s="8"/>
       <c r="T36" s="8"/>
     </row>
-    <row r="37" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>20</v>
       </c>
@@ -1690,7 +1690,7 @@
       <c r="I37" s="8"/>
       <c r="J37" s="14"/>
       <c r="K37" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L37" s="8"/>
       <c r="M37" s="8"/>
@@ -1701,7 +1701,7 @@
       <c r="S37" s="8"/>
       <c r="T37" s="8"/>
     </row>
-    <row r="38" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>22</v>
       </c>
@@ -1728,7 +1728,7 @@
       <c r="S38" s="8"/>
       <c r="T38" s="8"/>
     </row>
-    <row r="39" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>24</v>
       </c>
@@ -1749,7 +1749,7 @@
       <c r="L39" s="8"/>
       <c r="M39" s="14"/>
       <c r="N39" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O39" s="8"/>
       <c r="P39" s="8"/>
@@ -1757,7 +1757,7 @@
       <c r="S39" s="8"/>
       <c r="T39" s="8"/>
     </row>
-    <row r="40" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>17</v>
       </c>
@@ -1774,7 +1774,7 @@
       <c r="H40" s="13"/>
       <c r="I40" s="13"/>
       <c r="J40" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K40" s="8"/>
       <c r="L40" s="8"/>
@@ -1785,7 +1785,7 @@
       <c r="S40" s="8"/>
       <c r="T40" s="8"/>
     </row>
-    <row r="41" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>25</v>
       </c>
@@ -1807,14 +1807,14 @@
       <c r="M41"/>
       <c r="N41" s="11"/>
       <c r="O41" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P41" s="8"/>
       <c r="Q41" s="8"/>
       <c r="S41" s="8"/>
       <c r="T41" s="8"/>
     </row>
-    <row r="42" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>26</v>
       </c>
@@ -1836,14 +1836,14 @@
       <c r="M42"/>
       <c r="N42" s="11"/>
       <c r="O42" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P42" s="8"/>
       <c r="Q42" s="8"/>
       <c r="S42" s="8"/>
       <c r="T42" s="8"/>
     </row>
-    <row r="43" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>27</v>
       </c>
@@ -1870,7 +1870,7 @@
       <c r="S43" s="8"/>
       <c r="T43" s="8"/>
     </row>
-    <row r="44" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>28</v>
       </c>
@@ -1890,7 +1890,7 @@
       <c r="K44" s="12"/>
       <c r="L44" s="12"/>
       <c r="M44" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N44" s="8"/>
       <c r="O44" s="8"/>
@@ -1900,9 +1900,9 @@
       <c r="S44" s="8"/>
       <c r="T44" s="8"/>
     </row>
-    <row r="45" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>33</v>
@@ -1920,7 +1920,7 @@
       <c r="K45" s="17"/>
       <c r="L45" s="17"/>
       <c r="M45" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N45" s="8"/>
       <c r="O45" s="8"/>
@@ -1930,7 +1930,7 @@
       <c r="S45" s="8"/>
       <c r="T45" s="8"/>
     </row>
-    <row r="46" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>29</v>
       </c>
@@ -1950,7 +1950,7 @@
       <c r="K46" s="12"/>
       <c r="L46" s="12"/>
       <c r="M46" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N46" s="8"/>
       <c r="O46" s="8"/>
@@ -1960,7 +1960,7 @@
       <c r="S46" s="8"/>
       <c r="T46" s="8"/>
     </row>
-    <row r="47" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>49</v>
       </c>
@@ -1988,7 +1988,7 @@
       <c r="S47" s="8"/>
       <c r="T47" s="8"/>
     </row>
-    <row r="48" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>50</v>
       </c>
@@ -2000,7 +2000,7 @@
       </c>
       <c r="D48" s="10"/>
       <c r="E48" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
@@ -2018,9 +2018,9 @@
       <c r="S48" s="8"/>
       <c r="T48" s="8"/>
     </row>
-    <row r="49" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>33</v>
@@ -2031,7 +2031,7 @@
       <c r="D49" s="8"/>
       <c r="E49" s="11"/>
       <c r="F49" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G49" s="8"/>
       <c r="H49" s="8"/>
@@ -2048,9 +2048,9 @@
       <c r="S49" s="8"/>
       <c r="T49" s="8"/>
     </row>
-    <row r="50" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>33</v>
@@ -2060,11 +2060,11 @@
       </c>
       <c r="E50" s="14"/>
       <c r="F50" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P50" s="8"/>
     </row>
-    <row r="51" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G51" s="8"/>
       <c r="H51" s="8"/>
       <c r="I51" s="8"/>

</xml_diff>

<commit_message>
Update Usecase Format, Activity Diagram
Các chức năng: Chấm công, Quản lí danh mục, Báo cáo, Tìm kiếm, Quản lí kho
</commit_message>
<xml_diff>
--- a/Phân tích/Barchart.xlsx
+++ b/Phân tích/Barchart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CNPM\Phân tích\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Homework\CN Phan Mem\Homework\CNPM\Phân tích\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29CB8E90-D67C-45E4-A552-992AD8B20780}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48871916-9C8A-45AD-9265-4742BFD636E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -701,17 +701,17 @@
       <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="4" width="9.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="16" width="9.140625" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="29.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="1"/>
+    <col min="3" max="4" width="9.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="1"/>
+    <col min="6" max="16" width="9.109375" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>30</v>
       </c>
@@ -720,7 +720,7 @@
       <c r="D1" s="20"/>
       <c r="E1" s="20"/>
     </row>
-    <row r="2" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D2" s="5"/>
       <c r="E2" s="21" t="s">
         <v>46</v>
@@ -744,7 +744,7 @@
       <c r="R2"/>
       <c r="S2"/>
     </row>
-    <row r="3" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D3" s="7" t="s">
         <v>41</v>
       </c>
@@ -789,7 +789,7 @@
       <c r="S3" s="6"/>
       <c r="T3" s="6"/>
     </row>
-    <row r="4" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>31</v>
       </c>
@@ -798,7 +798,7 @@
       </c>
       <c r="O4"/>
     </row>
-    <row r="5" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -825,7 +825,7 @@
       <c r="S5" s="8"/>
       <c r="T5" s="8"/>
     </row>
-    <row r="6" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -854,7 +854,7 @@
       <c r="S6" s="8"/>
       <c r="T6" s="8"/>
     </row>
-    <row r="7" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -883,7 +883,7 @@
       <c r="S7" s="8"/>
       <c r="T7" s="8"/>
     </row>
-    <row r="8" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -912,7 +912,7 @@
       <c r="S8" s="8"/>
       <c r="T8" s="8"/>
     </row>
-    <row r="9" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19" t="s">
         <v>59</v>
       </c>
@@ -939,7 +939,7 @@
       <c r="S9" s="8"/>
       <c r="T9" s="8"/>
     </row>
-    <row r="10" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>60</v>
       </c>
@@ -958,7 +958,7 @@
       <c r="S10" s="8"/>
       <c r="T10" s="8"/>
     </row>
-    <row r="11" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>61</v>
       </c>
@@ -977,7 +977,7 @@
       <c r="S11" s="8"/>
       <c r="T11" s="8"/>
     </row>
-    <row r="12" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>58</v>
       </c>
@@ -996,7 +996,7 @@
       <c r="S12" s="8"/>
       <c r="T12" s="8"/>
     </row>
-    <row r="13" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -1022,7 +1022,7 @@
       <c r="S13" s="8"/>
       <c r="T13" s="8"/>
     </row>
-    <row r="14" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -1050,7 +1050,7 @@
       <c r="S14" s="8"/>
       <c r="T14" s="8"/>
     </row>
-    <row r="15" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>56</v>
       </c>
@@ -1078,7 +1078,7 @@
       <c r="S15" s="8"/>
       <c r="T15" s="8"/>
     </row>
-    <row r="16" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -1106,7 +1106,7 @@
       <c r="S16" s="8"/>
       <c r="T16" s="8"/>
     </row>
-    <row r="17" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -1134,7 +1134,7 @@
       <c r="S17" s="8"/>
       <c r="T17" s="8"/>
     </row>
-    <row r="18" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
@@ -1162,7 +1162,7 @@
       <c r="S18" s="8"/>
       <c r="T18" s="8"/>
     </row>
-    <row r="19" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>63</v>
       </c>
@@ -1191,7 +1191,7 @@
       <c r="S19" s="8"/>
       <c r="T19" s="8"/>
     </row>
-    <row r="20" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
@@ -1217,7 +1217,7 @@
       <c r="S20" s="8"/>
       <c r="T20" s="8"/>
     </row>
-    <row r="21" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
@@ -1245,7 +1245,7 @@
       <c r="S21" s="8"/>
       <c r="T21" s="8"/>
     </row>
-    <row r="22" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
@@ -1273,7 +1273,7 @@
       <c r="S22" s="8"/>
       <c r="T22" s="8"/>
     </row>
-    <row r="23" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>10</v>
       </c>
@@ -1301,7 +1301,7 @@
       <c r="S23" s="8"/>
       <c r="T23" s="8"/>
     </row>
-    <row r="24" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
@@ -1328,7 +1328,7 @@
       <c r="S24" s="8"/>
       <c r="T24" s="8"/>
     </row>
-    <row r="25" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
@@ -1357,7 +1357,7 @@
       <c r="S25" s="8"/>
       <c r="T25" s="8"/>
     </row>
-    <row r="26" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
@@ -1386,7 +1386,7 @@
       <c r="S26" s="8"/>
       <c r="T26" s="8"/>
     </row>
-    <row r="27" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
@@ -1415,7 +1415,7 @@
       <c r="S27" s="8"/>
       <c r="T27" s="8"/>
     </row>
-    <row r="28" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>5</v>
       </c>
@@ -1444,7 +1444,7 @@
       <c r="S28" s="8"/>
       <c r="T28" s="8"/>
     </row>
-    <row r="29" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>23</v>
       </c>
@@ -1473,7 +1473,7 @@
       <c r="S29" s="8"/>
       <c r="T29" s="8"/>
     </row>
-    <row r="30" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>3</v>
       </c>
@@ -1500,7 +1500,7 @@
       <c r="S30" s="8"/>
       <c r="T30" s="8"/>
     </row>
-    <row r="31" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>13</v>
       </c>
@@ -1529,7 +1529,7 @@
       <c r="S31" s="8"/>
       <c r="T31" s="8"/>
     </row>
-    <row r="32" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>21</v>
       </c>
@@ -1558,7 +1558,7 @@
       <c r="S32" s="8"/>
       <c r="T32" s="8"/>
     </row>
-    <row r="33" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>14</v>
       </c>
@@ -1587,7 +1587,7 @@
       <c r="S33" s="8"/>
       <c r="T33" s="8"/>
     </row>
-    <row r="34" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>15</v>
       </c>
@@ -1614,7 +1614,7 @@
       <c r="S34" s="8"/>
       <c r="T34" s="8"/>
     </row>
-    <row r="35" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>16</v>
       </c>
@@ -1643,7 +1643,7 @@
       <c r="S35" s="8"/>
       <c r="T35" s="8"/>
     </row>
-    <row r="36" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>18</v>
       </c>
@@ -1672,7 +1672,7 @@
       <c r="S36" s="8"/>
       <c r="T36" s="8"/>
     </row>
-    <row r="37" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>20</v>
       </c>
@@ -1701,7 +1701,7 @@
       <c r="S37" s="8"/>
       <c r="T37" s="8"/>
     </row>
-    <row r="38" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>22</v>
       </c>
@@ -1728,7 +1728,7 @@
       <c r="S38" s="8"/>
       <c r="T38" s="8"/>
     </row>
-    <row r="39" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>24</v>
       </c>
@@ -1757,7 +1757,7 @@
       <c r="S39" s="8"/>
       <c r="T39" s="8"/>
     </row>
-    <row r="40" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>17</v>
       </c>
@@ -1785,7 +1785,7 @@
       <c r="S40" s="8"/>
       <c r="T40" s="8"/>
     </row>
-    <row r="41" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>25</v>
       </c>
@@ -1814,7 +1814,7 @@
       <c r="S41" s="8"/>
       <c r="T41" s="8"/>
     </row>
-    <row r="42" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>26</v>
       </c>
@@ -1843,7 +1843,7 @@
       <c r="S42" s="8"/>
       <c r="T42" s="8"/>
     </row>
-    <row r="43" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>27</v>
       </c>
@@ -1870,7 +1870,7 @@
       <c r="S43" s="8"/>
       <c r="T43" s="8"/>
     </row>
-    <row r="44" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>28</v>
       </c>
@@ -1900,7 +1900,7 @@
       <c r="S44" s="8"/>
       <c r="T44" s="8"/>
     </row>
-    <row r="45" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>64</v>
       </c>
@@ -1930,7 +1930,7 @@
       <c r="S45" s="8"/>
       <c r="T45" s="8"/>
     </row>
-    <row r="46" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>29</v>
       </c>
@@ -1960,7 +1960,7 @@
       <c r="S46" s="8"/>
       <c r="T46" s="8"/>
     </row>
-    <row r="47" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>49</v>
       </c>
@@ -1988,7 +1988,7 @@
       <c r="S47" s="8"/>
       <c r="T47" s="8"/>
     </row>
-    <row r="48" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>50</v>
       </c>
@@ -2018,7 +2018,7 @@
       <c r="S48" s="8"/>
       <c r="T48" s="8"/>
     </row>
-    <row r="49" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>65</v>
       </c>
@@ -2048,7 +2048,7 @@
       <c r="S49" s="8"/>
       <c r="T49" s="8"/>
     </row>
-    <row r="50" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>62</v>
       </c>
@@ -2064,7 +2064,7 @@
       </c>
       <c r="P50" s="8"/>
     </row>
-    <row r="51" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G51" s="8"/>
       <c r="H51" s="8"/>
       <c r="I51" s="8"/>

</xml_diff>

<commit_message>
Tạo Slide thuyết trình, Đồ án
</commit_message>
<xml_diff>
--- a/Phân tích/Barchart.xlsx
+++ b/Phân tích/Barchart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Homework\CN Phan Mem\Homework\CNPM\Phân tích\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48871916-9C8A-45AD-9265-4742BFD636E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB01D7A5-0719-47B1-BB22-89F71CBEE22B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="66">
   <si>
     <t>Quản lí nhân viên</t>
   </si>
@@ -697,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="G60" sqref="G60"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -790,12 +790,8 @@
       <c r="T3" s="6"/>
     </row>
     <row r="4" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
       <c r="O4"/>
     </row>
     <row r="5" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
@@ -2084,7 +2080,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="C4 E3:P3" numberStoredAsText="1"/>
+    <ignoredError sqref="E3:P3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>